<commit_message>
Añadidos archivos de práctica y módulos aprendidos: funciones estadísticas, fecha y hora, texto, gráficos. Incluye ejercicios de los niveles básico e intermedio y el archivo de Ventas 2024. Avance registrado del proceso de aprendizaje.
</commit_message>
<xml_diff>
--- a/NivelBasico/Módulo 7 - Funciones Estadísticas.xlsx
+++ b/NivelBasico/Módulo 7 - Funciones Estadísticas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\db\Nik Denilson\Cursos\EXCEL\NivelBasico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3B8F44-A6D3-4141-B31B-FB70B147B2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B5C41-A441-4EA3-9304-46417AD017A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="787" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="787" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="101" r:id="rId1"/>
@@ -7419,8 +7419,8 @@
   </sheetPr>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:E8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1"/>
@@ -7777,7 +7777,7 @@
   </sheetPr>
   <dimension ref="B1:N434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
@@ -8993,8 +8993,8 @@
   </sheetPr>
   <dimension ref="B1:N440"/>
   <sheetViews>
-    <sheetView topLeftCell="C110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M110" sqref="M110"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>

</xml_diff>